<commit_message>
+ send invoice by email and also added the docker file to allow the app to run in docker/ kubernetes/ openShift
</commit_message>
<xml_diff>
--- a/suppliers/anothercompany/customer.xlsx
+++ b/suppliers/anothercompany/customer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianrentea/Desktop/generate-invoice/furnizori/anothercompany/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianrentea/Documents/GitHub/invoicing-app/suppliers/anothercompany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84287D24-F574-5B4D-B7DE-9E334AC47FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0627A7-1EB9-374D-BAC4-1F4B56A25384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="27640" windowHeight="15900" xr2:uid="{CB570BF5-8DF4-9B4D-997E-E805A1D9601E}"/>
+    <workbookView xWindow="780" yWindow="520" windowWidth="27640" windowHeight="15900" xr2:uid="{CB570BF5-8DF4-9B4D-997E-E805A1D9601E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CIF</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>RO89INGB550199991132209</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>adrianrentea01@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372BB633-41A5-E841-8692-3FF565AF51A2}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,9 +444,10 @@
     <col min="4" max="4" width="57.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -462,8 +469,11 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -484,6 +494,9 @@
       </c>
       <c r="G2">
         <v>29999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>